<commit_message>
Pushed on 12/8/2022 (Stable)
</commit_message>
<xml_diff>
--- a/KohlerAutomation/Data/Cost.xlsx
+++ b/KohlerAutomation/Data/Cost.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>#</t>
   </si>
@@ -28,79 +28,64 @@
     <t>15399T-B-BV</t>
   </si>
   <si>
-    <t>Rs.8,010.00</t>
-  </si>
-  <si>
     <t>5171T-CM-0</t>
   </si>
   <si>
     <t>29959IN-BV</t>
   </si>
   <si>
-    <t>Rs.155,000.00</t>
+    <t>17629IN-SM-0</t>
   </si>
   <si>
-    <t>17629IN-SM-0</t>
+    <t>20742IN-9FP-RGD</t>
+  </si>
+  <si>
+    <t>16817IN-2SR-0</t>
+  </si>
+  <si>
+    <t>31014IN-0</t>
+  </si>
+  <si>
+    <t>29583IN-4-CP</t>
+  </si>
+  <si>
+    <t>11543IN-4-AF</t>
+  </si>
+  <si>
+    <t>29584IN-4-CP</t>
+  </si>
+  <si>
+    <t>77142IN-S-HP1</t>
+  </si>
+  <si>
+    <t>29017IN-SS-0</t>
+  </si>
+  <si>
+    <t>20742IN-9FP-CP</t>
+  </si>
+  <si>
+    <t>99966IN-4-CP</t>
+  </si>
+  <si>
+    <t>9301T-ZX-BV</t>
+  </si>
+  <si>
+    <t>72796T-CP</t>
   </si>
   <si>
     <t>20742IN-9FP-BL</t>
   </si>
   <si>
-    <t>Rs.14,700.00</t>
-  </si>
-  <si>
-    <t>16817IN-2SR-0</t>
-  </si>
-  <si>
-    <t>20742IN-9FP-RGD</t>
-  </si>
-  <si>
-    <t>Rs.15,800.00</t>
-  </si>
-  <si>
-    <t>29583IN-4-CP</t>
-  </si>
-  <si>
-    <t>31014IN-0</t>
-  </si>
-  <si>
-    <t>Rs.83,750.00</t>
-  </si>
-  <si>
-    <t>29584IN-4-CP</t>
-  </si>
-  <si>
-    <t>11543IN-4-AF</t>
-  </si>
-  <si>
-    <t>Rs.5,330.00</t>
-  </si>
-  <si>
-    <t>29017IN-SS-0</t>
-  </si>
-  <si>
-    <t>77142IN-S-HP1</t>
-  </si>
-  <si>
-    <t>Product Not Found</t>
-  </si>
-  <si>
-    <t>99966IN-4-CP</t>
-  </si>
-  <si>
-    <t>20742IN-9FP-CP</t>
-  </si>
-  <si>
-    <t>Rs.10,500.00</t>
-  </si>
-  <si>
-    <t>72796T-CP</t>
-  </si>
-  <si>
     <t>29992IN-CP</t>
   </si>
   <si>
+    <t>33932IN-0</t>
+  </si>
+  <si>
     <t>72568T-CP</t>
+  </si>
+  <si>
+    <t>33933IN-0</t>
   </si>
   <si>
     <t>72572T-CP</t>
@@ -154,16 +139,7 @@
     <t>30375IN-0</t>
   </si>
   <si>
-    <t>9301T-ZX-BV</t>
-  </si>
-  <si>
     <t>9301T-ZX-RGD</t>
-  </si>
-  <si>
-    <t>33932IN-0</t>
-  </si>
-  <si>
-    <t>33933IN-0</t>
   </si>
 </sst>
 </file>
@@ -171,10 +147,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -205,9 +181,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -220,24 +217,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -250,7 +232,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,6 +247,14 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
@@ -273,24 +263,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -310,15 +285,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,7 +310,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -342,7 +318,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,7 +358,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,31 +448,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,139 +532,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,23 +585,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,15 +615,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -674,6 +626,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,148 +682,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1148,14 +1124,14 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" customWidth="true" style="1" width="14.8571428571429" collapsed="true"/>
-    <col min="3" max="3" style="2" width="12.6285714285714" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="21.8571428571429" collapsed="true"/>
+    <col min="2" max="2" width="14.8571428571429" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6285714285714" style="2"/>
+    <col min="4" max="4" width="21.8571428571429" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
@@ -1176,12 +1152,10 @@
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
+      <c r="D2"/>
       <c r="J2" s="8"/>
       <c r="K2" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:11">
@@ -1189,63 +1163,55 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D3"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:11">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>9</v>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
+      <c r="D4"/>
       <c r="J4" s="8"/>
       <c r="K4" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:11">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
+      <c r="D5"/>
       <c r="J5" s="1"/>
       <c r="K5" s="10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:11">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>15</v>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
+      <c r="D6"/>
       <c r="J6" s="8"/>
       <c r="K6" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:11">
@@ -1253,15 +1219,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D7"/>
       <c r="J7" s="1"/>
       <c r="K7" s="10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:11">
@@ -1269,61 +1233,66 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
+      <c r="D8"/>
       <c r="J8" s="1"/>
       <c r="K8" s="10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:11">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
+      <c r="B9" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
+      <c r="D9"/>
       <c r="J9" s="1"/>
       <c r="K9" s="10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:11">
       <c r="A10" s="7">
         <v>9</v>
       </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10"/>
       <c r="K10" s="10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:11">
       <c r="A11" s="7">
         <v>10</v>
       </c>
+      <c r="B11" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="9"/>
       <c r="D11"/>
       <c r="K11" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:11">
       <c r="A12" s="7">
         <v>11</v>
       </c>
+      <c r="B12" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="C12" s="9"/>
       <c r="D12"/>
       <c r="K12" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:11">
@@ -1333,7 +1302,7 @@
       <c r="C13" s="9"/>
       <c r="D13"/>
       <c r="K13" s="10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:11">
@@ -1343,7 +1312,7 @@
       <c r="C14" s="9"/>
       <c r="D14"/>
       <c r="K14" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:11">
@@ -1353,7 +1322,7 @@
       <c r="C15" s="9"/>
       <c r="D15"/>
       <c r="K15" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:11">
@@ -1363,7 +1332,7 @@
       <c r="C16" s="9"/>
       <c r="D16"/>
       <c r="K16" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:11">
@@ -1372,7 +1341,7 @@
       </c>
       <c r="C17" s="9"/>
       <c r="K17" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:11">
@@ -1381,7 +1350,7 @@
       </c>
       <c r="C18" s="9"/>
       <c r="K18" s="10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:11">
@@ -1390,7 +1359,7 @@
       </c>
       <c r="C19" s="9"/>
       <c r="K19" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:11">
@@ -1399,7 +1368,7 @@
       </c>
       <c r="C20" s="9"/>
       <c r="K20" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:11">
@@ -1408,7 +1377,7 @@
       </c>
       <c r="C21" s="9"/>
       <c r="K21" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:11">
@@ -1417,7 +1386,7 @@
       </c>
       <c r="C22" s="9"/>
       <c r="K22" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:11">
@@ -1426,7 +1395,7 @@
       </c>
       <c r="C23" s="9"/>
       <c r="K23" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:11">
@@ -1435,7 +1404,7 @@
       </c>
       <c r="C24" s="9"/>
       <c r="K24" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:11">
@@ -1444,7 +1413,7 @@
       </c>
       <c r="C25" s="9"/>
       <c r="K25" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:11">
@@ -1453,7 +1422,7 @@
       </c>
       <c r="C26" s="9"/>
       <c r="K26" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:11">
@@ -1462,7 +1431,7 @@
       </c>
       <c r="C27" s="9"/>
       <c r="K27" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:11">
@@ -1471,7 +1440,7 @@
       </c>
       <c r="C28" s="9"/>
       <c r="K28" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:11">
@@ -1480,7 +1449,7 @@
       </c>
       <c r="C29" s="9"/>
       <c r="K29" s="10" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:11">
@@ -1489,7 +1458,7 @@
       </c>
       <c r="C30" s="9"/>
       <c r="K30" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:11">
@@ -1498,7 +1467,7 @@
       </c>
       <c r="C31" s="9"/>
       <c r="K31" s="11" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:11">
@@ -1507,7 +1476,7 @@
       </c>
       <c r="C32" s="9"/>
       <c r="K32" s="11" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:3">

</xml_diff>